<commit_message>
Changelog: - CORE: -- trades.cost_group removed -- job.cost_group added - OUPUT: -- templates refined -- cost_group_ov unfinished
</commit_message>
<xml_diff>
--- a/templates/trades_ov.xlsx
+++ b/templates/trades_ov.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Google Drive\02 Arbeit\00 Fyuture\01 Learning\Python\00 Projekte\Kostenfortschreibung\Application\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59AF22DE-2468-49EB-999B-856B031858D2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{333716FE-A9E5-4BBF-9620-5ADC628326C4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FB0F6570-8FBC-4219-A065-E08E6DA1902A}"/>
+    <workbookView xWindow="7770" yWindow="2835" windowWidth="38700" windowHeight="15435" xr2:uid="{FB0F6570-8FBC-4219-A065-E08E6DA1902A}"/>
   </bookViews>
   <sheets>
     <sheet name="TEMPLATE" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
   <definedNames>
     <definedName name="Auftragsnummern">[1]!Auftrag[Aufträge]</definedName>
     <definedName name="Betrag">[1]Rechnungsprüfung!$I$15:$J$24</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">TEMPLATE!$A$1:$E$31</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">TEMPLATE!$A$1:$F$31</definedName>
     <definedName name="Gewerk">'[1]Aufträge-Gewerk'!$F$2</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -243,13 +243,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>7</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>1209547</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>180975</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>2232468</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>318684</xdr:rowOff>
@@ -638,26 +638,27 @@
   <sheetPr codeName="Tabelle1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:H72"/>
+  <dimension ref="A1:I72"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:G1048576"/>
+      <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.28515625" style="4" customWidth="1"/>
+    <col min="1" max="1" width="20" style="4" customWidth="1"/>
     <col min="2" max="2" width="23.7109375" style="4" customWidth="1"/>
-    <col min="3" max="3" width="17.85546875" style="4" customWidth="1"/>
-    <col min="4" max="4" width="23" style="4" customWidth="1"/>
-    <col min="5" max="5" width="36.7109375" style="4" customWidth="1"/>
-    <col min="6" max="6" width="23.28515625" style="4" customWidth="1"/>
-    <col min="7" max="7" width="36.140625" style="4" customWidth="1"/>
-    <col min="8" max="8" width="33.7109375" style="4" customWidth="1"/>
-    <col min="9" max="16384" width="11.42578125" style="4"/>
+    <col min="3" max="3" width="13.7109375" style="4" customWidth="1"/>
+    <col min="4" max="4" width="15" style="4" customWidth="1"/>
+    <col min="5" max="5" width="23" style="4" customWidth="1"/>
+    <col min="6" max="6" width="36.7109375" style="4" customWidth="1"/>
+    <col min="7" max="7" width="23.28515625" style="4" customWidth="1"/>
+    <col min="8" max="8" width="36.140625" style="4" customWidth="1"/>
+    <col min="9" max="9" width="33.7109375" style="4" customWidth="1"/>
+    <col min="10" max="16384" width="11.42578125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="3" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="3" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="13"/>
       <c r="B1" s="13"/>
       <c r="C1" s="13"/>
@@ -666,13 +667,14 @@
       <c r="F1" s="13"/>
       <c r="G1" s="13"/>
       <c r="H1" s="13"/>
-    </row>
-    <row r="2" spans="1:8" ht="22.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I1" s="13"/>
+    </row>
+    <row r="2" spans="1:9" ht="22.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="14" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>1</v>
       </c>
@@ -680,7 +682,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>2</v>
       </c>
@@ -688,7 +690,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="69" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="69" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="16" t="s">
         <v>3</v>
       </c>
@@ -696,21 +698,22 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="62.65" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:9" ht="62.65" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B6" s="17" t="s">
         <v>4</v>
       </c>
       <c r="C6" s="17"/>
       <c r="D6" s="17"/>
       <c r="E6" s="17"/>
-    </row>
-    <row r="7" spans="1:8" ht="29.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="F6" s="17"/>
+    </row>
+    <row r="7" spans="1:9" ht="29.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="2"/>
       <c r="B7" s="3"/>
-      <c r="D7" s="2"/>
       <c r="E7" s="2"/>
-    </row>
-    <row r="8" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F7" s="2"/>
+    </row>
+    <row r="8" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5"/>
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
@@ -719,118 +722,130 @@
       <c r="F8" s="5"/>
       <c r="G8" s="5"/>
       <c r="H8" s="5"/>
-    </row>
-    <row r="9" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I8" s="5"/>
+    </row>
+    <row r="9" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="6"/>
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
       <c r="D9" s="6"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="5"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="7"/>
       <c r="G9" s="5"/>
       <c r="H9" s="5"/>
-    </row>
-    <row r="10" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I9" s="5"/>
+    </row>
+    <row r="10" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="6"/>
       <c r="B10" s="8"/>
       <c r="C10" s="8"/>
       <c r="D10" s="8"/>
       <c r="E10" s="8"/>
-      <c r="F10" s="9"/>
+      <c r="F10" s="8"/>
       <c r="G10" s="9"/>
-      <c r="H10" s="5"/>
-    </row>
-    <row r="11" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H10" s="9"/>
+      <c r="I10" s="5"/>
+    </row>
+    <row r="11" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="6"/>
       <c r="B11" s="6"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
-      <c r="F11" s="5"/>
+      <c r="F11" s="1"/>
       <c r="G11" s="5"/>
       <c r="H11" s="5"/>
-    </row>
-    <row r="12" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I11" s="5"/>
+    </row>
+    <row r="12" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="6"/>
       <c r="B12" s="10"/>
       <c r="C12" s="10"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="5"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="6"/>
       <c r="G12" s="5"/>
       <c r="H12" s="5"/>
-    </row>
-    <row r="13" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I12" s="5"/>
+    </row>
+    <row r="13" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="6"/>
       <c r="B13" s="6"/>
       <c r="C13" s="8"/>
       <c r="D13" s="8"/>
       <c r="E13" s="8"/>
-      <c r="F13" s="11"/>
+      <c r="F13" s="8"/>
       <c r="G13" s="11"/>
-      <c r="H13" s="5"/>
-    </row>
-    <row r="14" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H13" s="11"/>
+      <c r="I13" s="5"/>
+    </row>
+    <row r="14" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="6"/>
       <c r="B14" s="6"/>
       <c r="C14" s="8"/>
       <c r="D14" s="8"/>
       <c r="E14" s="8"/>
-      <c r="F14" s="11"/>
+      <c r="F14" s="8"/>
       <c r="G14" s="11"/>
-      <c r="H14" s="5"/>
-    </row>
-    <row r="15" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H14" s="11"/>
+      <c r="I14" s="5"/>
+    </row>
+    <row r="15" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="6"/>
       <c r="B15" s="6"/>
       <c r="C15" s="8"/>
       <c r="D15" s="8"/>
       <c r="E15" s="8"/>
-      <c r="F15" s="11"/>
+      <c r="F15" s="8"/>
       <c r="G15" s="11"/>
-      <c r="H15" s="5"/>
-    </row>
-    <row r="16" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H15" s="11"/>
+      <c r="I15" s="5"/>
+    </row>
+    <row r="16" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="6"/>
       <c r="B16" s="6"/>
       <c r="C16" s="8"/>
       <c r="D16" s="8"/>
       <c r="E16" s="8"/>
-      <c r="F16" s="11"/>
+      <c r="F16" s="8"/>
       <c r="G16" s="11"/>
-      <c r="H16" s="5"/>
-    </row>
-    <row r="17" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H16" s="11"/>
+      <c r="I16" s="5"/>
+    </row>
+    <row r="17" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="6"/>
       <c r="B17" s="8"/>
       <c r="C17" s="8"/>
       <c r="D17" s="8"/>
       <c r="E17" s="8"/>
-      <c r="F17" s="11"/>
+      <c r="F17" s="8"/>
       <c r="G17" s="11"/>
-      <c r="H17" s="5"/>
-    </row>
-    <row r="18" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H17" s="11"/>
+      <c r="I17" s="5"/>
+    </row>
+    <row r="18" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="6"/>
       <c r="B18" s="8"/>
       <c r="C18" s="8"/>
       <c r="D18" s="8"/>
       <c r="E18" s="8"/>
-      <c r="F18" s="11"/>
+      <c r="F18" s="8"/>
       <c r="G18" s="11"/>
-      <c r="H18" s="5"/>
-    </row>
-    <row r="19" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H18" s="11"/>
+      <c r="I18" s="5"/>
+    </row>
+    <row r="19" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="5"/>
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
       <c r="D19" s="5"/>
       <c r="E19" s="5"/>
-      <c r="F19" s="11"/>
+      <c r="F19" s="5"/>
       <c r="G19" s="11"/>
-      <c r="H19" s="5"/>
-    </row>
-    <row r="20" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H19" s="11"/>
+      <c r="I19" s="5"/>
+    </row>
+    <row r="20" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="5"/>
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
@@ -839,8 +854,9 @@
       <c r="F20" s="5"/>
       <c r="G20" s="5"/>
       <c r="H20" s="5"/>
-    </row>
-    <row r="21" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I20" s="5"/>
+    </row>
+    <row r="21" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="5"/>
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
@@ -849,18 +865,20 @@
       <c r="F21" s="5"/>
       <c r="G21" s="5"/>
       <c r="H21" s="5"/>
-    </row>
-    <row r="22" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I21" s="5"/>
+    </row>
+    <row r="22" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="5"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
-      <c r="E22" s="12"/>
-      <c r="F22" s="5"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="12"/>
       <c r="G22" s="5"/>
       <c r="H22" s="5"/>
-    </row>
-    <row r="23" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I22" s="5"/>
+    </row>
+    <row r="23" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="5"/>
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
@@ -869,8 +887,9 @@
       <c r="F23" s="5"/>
       <c r="G23" s="5"/>
       <c r="H23" s="5"/>
-    </row>
-    <row r="24" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I23" s="5"/>
+    </row>
+    <row r="24" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="5"/>
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
@@ -879,8 +898,9 @@
       <c r="F24" s="5"/>
       <c r="G24" s="5"/>
       <c r="H24" s="5"/>
-    </row>
-    <row r="25" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I24" s="5"/>
+    </row>
+    <row r="25" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="5"/>
       <c r="B25" s="5"/>
       <c r="C25" s="5"/>
@@ -889,8 +909,9 @@
       <c r="F25" s="5"/>
       <c r="G25" s="5"/>
       <c r="H25" s="5"/>
-    </row>
-    <row r="26" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I25" s="5"/>
+    </row>
+    <row r="26" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="5"/>
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
@@ -899,8 +920,9 @@
       <c r="F26" s="5"/>
       <c r="G26" s="5"/>
       <c r="H26" s="5"/>
-    </row>
-    <row r="27" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I26" s="5"/>
+    </row>
+    <row r="27" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="5"/>
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
@@ -909,8 +931,9 @@
       <c r="F27" s="5"/>
       <c r="G27" s="5"/>
       <c r="H27" s="5"/>
-    </row>
-    <row r="28" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I27" s="5"/>
+    </row>
+    <row r="28" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="5"/>
       <c r="B28" s="5"/>
       <c r="C28" s="5"/>
@@ -919,8 +942,9 @@
       <c r="F28" s="5"/>
       <c r="G28" s="5"/>
       <c r="H28" s="5"/>
-    </row>
-    <row r="29" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I28" s="5"/>
+    </row>
+    <row r="29" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="5"/>
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
@@ -929,8 +953,9 @@
       <c r="F29" s="5"/>
       <c r="G29" s="5"/>
       <c r="H29" s="5"/>
-    </row>
-    <row r="30" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I29" s="5"/>
+    </row>
+    <row r="30" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="5"/>
       <c r="B30" s="5"/>
       <c r="C30" s="5"/>
@@ -939,8 +964,9 @@
       <c r="F30" s="5"/>
       <c r="G30" s="5"/>
       <c r="H30" s="5"/>
-    </row>
-    <row r="31" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I30" s="5"/>
+    </row>
+    <row r="31" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="5"/>
       <c r="B31" s="5"/>
       <c r="C31" s="5"/>
@@ -949,8 +975,9 @@
       <c r="F31" s="5"/>
       <c r="G31" s="5"/>
       <c r="H31" s="5"/>
-    </row>
-    <row r="32" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I31" s="5"/>
+    </row>
+    <row r="32" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="5"/>
       <c r="B32" s="5"/>
       <c r="C32" s="5"/>
@@ -959,8 +986,9 @@
       <c r="F32" s="5"/>
       <c r="G32" s="5"/>
       <c r="H32" s="5"/>
-    </row>
-    <row r="33" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="I32" s="5"/>
+    </row>
+    <row r="33" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A33" s="5"/>
       <c r="B33" s="5"/>
       <c r="C33" s="5"/>
@@ -969,8 +997,9 @@
       <c r="F33" s="5"/>
       <c r="G33" s="5"/>
       <c r="H33" s="5"/>
-    </row>
-    <row r="34" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="I33" s="5"/>
+    </row>
+    <row r="34" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A34" s="5"/>
       <c r="B34" s="5"/>
       <c r="C34" s="5"/>
@@ -979,8 +1008,9 @@
       <c r="F34" s="5"/>
       <c r="G34" s="5"/>
       <c r="H34" s="5"/>
-    </row>
-    <row r="35" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="I34" s="5"/>
+    </row>
+    <row r="35" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A35" s="5"/>
       <c r="B35" s="5"/>
       <c r="C35" s="5"/>
@@ -989,8 +1019,9 @@
       <c r="F35" s="5"/>
       <c r="G35" s="5"/>
       <c r="H35" s="5"/>
-    </row>
-    <row r="36" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="I35" s="5"/>
+    </row>
+    <row r="36" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A36" s="5"/>
       <c r="B36" s="5"/>
       <c r="C36" s="5"/>
@@ -999,8 +1030,9 @@
       <c r="F36" s="5"/>
       <c r="G36" s="5"/>
       <c r="H36" s="5"/>
-    </row>
-    <row r="37" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="I36" s="5"/>
+    </row>
+    <row r="37" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A37" s="5"/>
       <c r="B37" s="5"/>
       <c r="C37" s="5"/>
@@ -1009,8 +1041,9 @@
       <c r="F37" s="5"/>
       <c r="G37" s="5"/>
       <c r="H37" s="5"/>
-    </row>
-    <row r="38" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="I37" s="5"/>
+    </row>
+    <row r="38" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A38" s="5"/>
       <c r="B38" s="5"/>
       <c r="C38" s="5"/>
@@ -1019,8 +1052,9 @@
       <c r="F38" s="5"/>
       <c r="G38" s="5"/>
       <c r="H38" s="5"/>
-    </row>
-    <row r="39" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="I38" s="5"/>
+    </row>
+    <row r="39" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A39" s="5"/>
       <c r="B39" s="5"/>
       <c r="C39" s="5"/>
@@ -1029,8 +1063,9 @@
       <c r="F39" s="5"/>
       <c r="G39" s="5"/>
       <c r="H39" s="5"/>
-    </row>
-    <row r="40" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="I39" s="5"/>
+    </row>
+    <row r="40" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A40" s="5"/>
       <c r="B40" s="5"/>
       <c r="C40" s="5"/>
@@ -1039,8 +1074,9 @@
       <c r="F40" s="5"/>
       <c r="G40" s="5"/>
       <c r="H40" s="5"/>
-    </row>
-    <row r="41" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="I40" s="5"/>
+    </row>
+    <row r="41" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A41" s="5"/>
       <c r="B41" s="5"/>
       <c r="C41" s="5"/>
@@ -1049,8 +1085,9 @@
       <c r="F41" s="5"/>
       <c r="G41" s="5"/>
       <c r="H41" s="5"/>
-    </row>
-    <row r="42" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="I41" s="5"/>
+    </row>
+    <row r="42" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A42" s="5"/>
       <c r="B42" s="5"/>
       <c r="C42" s="5"/>
@@ -1059,8 +1096,9 @@
       <c r="F42" s="5"/>
       <c r="G42" s="5"/>
       <c r="H42" s="5"/>
-    </row>
-    <row r="43" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="I42" s="5"/>
+    </row>
+    <row r="43" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A43" s="5"/>
       <c r="B43" s="5"/>
       <c r="C43" s="5"/>
@@ -1069,8 +1107,9 @@
       <c r="F43" s="5"/>
       <c r="G43" s="5"/>
       <c r="H43" s="5"/>
-    </row>
-    <row r="44" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="I43" s="5"/>
+    </row>
+    <row r="44" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A44" s="5"/>
       <c r="B44" s="5"/>
       <c r="C44" s="5"/>
@@ -1079,8 +1118,9 @@
       <c r="F44" s="5"/>
       <c r="G44" s="5"/>
       <c r="H44" s="5"/>
-    </row>
-    <row r="45" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="I44" s="5"/>
+    </row>
+    <row r="45" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A45" s="5"/>
       <c r="B45" s="5"/>
       <c r="C45" s="5"/>
@@ -1089,8 +1129,9 @@
       <c r="F45" s="5"/>
       <c r="G45" s="5"/>
       <c r="H45" s="5"/>
-    </row>
-    <row r="46" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="I45" s="5"/>
+    </row>
+    <row r="46" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A46" s="5"/>
       <c r="B46" s="5"/>
       <c r="C46" s="5"/>
@@ -1099,8 +1140,9 @@
       <c r="F46" s="5"/>
       <c r="G46" s="5"/>
       <c r="H46" s="5"/>
-    </row>
-    <row r="47" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="I46" s="5"/>
+    </row>
+    <row r="47" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A47" s="5"/>
       <c r="B47" s="5"/>
       <c r="C47" s="5"/>
@@ -1109,8 +1151,9 @@
       <c r="F47" s="5"/>
       <c r="G47" s="5"/>
       <c r="H47" s="5"/>
-    </row>
-    <row r="48" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="I47" s="5"/>
+    </row>
+    <row r="48" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A48" s="5"/>
       <c r="B48" s="5"/>
       <c r="C48" s="5"/>
@@ -1119,8 +1162,9 @@
       <c r="F48" s="5"/>
       <c r="G48" s="5"/>
       <c r="H48" s="5"/>
-    </row>
-    <row r="49" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="I48" s="5"/>
+    </row>
+    <row r="49" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A49" s="5"/>
       <c r="B49" s="5"/>
       <c r="C49" s="5"/>
@@ -1129,8 +1173,9 @@
       <c r="F49" s="5"/>
       <c r="G49" s="5"/>
       <c r="H49" s="5"/>
-    </row>
-    <row r="50" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="I49" s="5"/>
+    </row>
+    <row r="50" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A50" s="5"/>
       <c r="B50" s="5"/>
       <c r="C50" s="5"/>
@@ -1139,8 +1184,9 @@
       <c r="F50" s="5"/>
       <c r="G50" s="5"/>
       <c r="H50" s="5"/>
-    </row>
-    <row r="51" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="I50" s="5"/>
+    </row>
+    <row r="51" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A51" s="5"/>
       <c r="B51" s="5"/>
       <c r="C51" s="5"/>
@@ -1149,8 +1195,9 @@
       <c r="F51" s="5"/>
       <c r="G51" s="5"/>
       <c r="H51" s="5"/>
-    </row>
-    <row r="52" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="I51" s="5"/>
+    </row>
+    <row r="52" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A52" s="5"/>
       <c r="B52" s="5"/>
       <c r="C52" s="5"/>
@@ -1159,8 +1206,9 @@
       <c r="F52" s="5"/>
       <c r="G52" s="5"/>
       <c r="H52" s="5"/>
-    </row>
-    <row r="53" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="I52" s="5"/>
+    </row>
+    <row r="53" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A53" s="5"/>
       <c r="B53" s="5"/>
       <c r="C53" s="5"/>
@@ -1169,8 +1217,9 @@
       <c r="F53" s="5"/>
       <c r="G53" s="5"/>
       <c r="H53" s="5"/>
-    </row>
-    <row r="54" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="I53" s="5"/>
+    </row>
+    <row r="54" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A54" s="5"/>
       <c r="B54" s="5"/>
       <c r="C54" s="5"/>
@@ -1179,8 +1228,9 @@
       <c r="F54" s="5"/>
       <c r="G54" s="5"/>
       <c r="H54" s="5"/>
-    </row>
-    <row r="55" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="I54" s="5"/>
+    </row>
+    <row r="55" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A55" s="5"/>
       <c r="B55" s="5"/>
       <c r="C55" s="5"/>
@@ -1189,8 +1239,9 @@
       <c r="F55" s="5"/>
       <c r="G55" s="5"/>
       <c r="H55" s="5"/>
-    </row>
-    <row r="56" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="I55" s="5"/>
+    </row>
+    <row r="56" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A56" s="5"/>
       <c r="B56" s="5"/>
       <c r="C56" s="5"/>
@@ -1199,8 +1250,9 @@
       <c r="F56" s="5"/>
       <c r="G56" s="5"/>
       <c r="H56" s="5"/>
-    </row>
-    <row r="57" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="I56" s="5"/>
+    </row>
+    <row r="57" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A57" s="5"/>
       <c r="B57" s="5"/>
       <c r="C57" s="5"/>
@@ -1209,8 +1261,9 @@
       <c r="F57" s="5"/>
       <c r="G57" s="5"/>
       <c r="H57" s="5"/>
-    </row>
-    <row r="58" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="I57" s="5"/>
+    </row>
+    <row r="58" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A58" s="5"/>
       <c r="B58" s="5"/>
       <c r="C58" s="5"/>
@@ -1219,8 +1272,9 @@
       <c r="F58" s="5"/>
       <c r="G58" s="5"/>
       <c r="H58" s="5"/>
-    </row>
-    <row r="59" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="I58" s="5"/>
+    </row>
+    <row r="59" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A59" s="5"/>
       <c r="B59" s="5"/>
       <c r="C59" s="5"/>
@@ -1229,8 +1283,9 @@
       <c r="F59" s="5"/>
       <c r="G59" s="5"/>
       <c r="H59" s="5"/>
-    </row>
-    <row r="60" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="I59" s="5"/>
+    </row>
+    <row r="60" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A60" s="5"/>
       <c r="B60" s="5"/>
       <c r="C60" s="5"/>
@@ -1239,8 +1294,9 @@
       <c r="F60" s="5"/>
       <c r="G60" s="5"/>
       <c r="H60" s="5"/>
-    </row>
-    <row r="61" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="I60" s="5"/>
+    </row>
+    <row r="61" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A61" s="5"/>
       <c r="B61" s="5"/>
       <c r="C61" s="5"/>
@@ -1249,8 +1305,9 @@
       <c r="F61" s="5"/>
       <c r="G61" s="5"/>
       <c r="H61" s="5"/>
-    </row>
-    <row r="62" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="I61" s="5"/>
+    </row>
+    <row r="62" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A62" s="5"/>
       <c r="B62" s="5"/>
       <c r="C62" s="5"/>
@@ -1259,8 +1316,9 @@
       <c r="F62" s="5"/>
       <c r="G62" s="5"/>
       <c r="H62" s="5"/>
-    </row>
-    <row r="63" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="I62" s="5"/>
+    </row>
+    <row r="63" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A63" s="5"/>
       <c r="B63" s="5"/>
       <c r="C63" s="5"/>
@@ -1269,8 +1327,9 @@
       <c r="F63" s="5"/>
       <c r="G63" s="5"/>
       <c r="H63" s="5"/>
-    </row>
-    <row r="64" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="I63" s="5"/>
+    </row>
+    <row r="64" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A64" s="5"/>
       <c r="B64" s="5"/>
       <c r="C64" s="5"/>
@@ -1279,8 +1338,9 @@
       <c r="F64" s="5"/>
       <c r="G64" s="5"/>
       <c r="H64" s="5"/>
-    </row>
-    <row r="65" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="I64" s="5"/>
+    </row>
+    <row r="65" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A65" s="5"/>
       <c r="B65" s="5"/>
       <c r="C65" s="5"/>
@@ -1289,8 +1349,9 @@
       <c r="F65" s="5"/>
       <c r="G65" s="5"/>
       <c r="H65" s="5"/>
-    </row>
-    <row r="66" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="I65" s="5"/>
+    </row>
+    <row r="66" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A66" s="5"/>
       <c r="B66" s="5"/>
       <c r="C66" s="5"/>
@@ -1299,8 +1360,9 @@
       <c r="F66" s="5"/>
       <c r="G66" s="5"/>
       <c r="H66" s="5"/>
-    </row>
-    <row r="67" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="I66" s="5"/>
+    </row>
+    <row r="67" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A67" s="5"/>
       <c r="B67" s="5"/>
       <c r="C67" s="5"/>
@@ -1309,8 +1371,9 @@
       <c r="F67" s="5"/>
       <c r="G67" s="5"/>
       <c r="H67" s="5"/>
-    </row>
-    <row r="68" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="I67" s="5"/>
+    </row>
+    <row r="68" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A68" s="5"/>
       <c r="B68" s="5"/>
       <c r="C68" s="5"/>
@@ -1319,8 +1382,9 @@
       <c r="F68" s="5"/>
       <c r="G68" s="5"/>
       <c r="H68" s="5"/>
-    </row>
-    <row r="69" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="I68" s="5"/>
+    </row>
+    <row r="69" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A69" s="5"/>
       <c r="B69" s="5"/>
       <c r="C69" s="5"/>
@@ -1329,8 +1393,9 @@
       <c r="F69" s="5"/>
       <c r="G69" s="5"/>
       <c r="H69" s="5"/>
-    </row>
-    <row r="70" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="I69" s="5"/>
+    </row>
+    <row r="70" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A70" s="5"/>
       <c r="B70" s="5"/>
       <c r="C70" s="5"/>
@@ -1339,8 +1404,9 @@
       <c r="F70" s="5"/>
       <c r="G70" s="5"/>
       <c r="H70" s="5"/>
-    </row>
-    <row r="71" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="I70" s="5"/>
+    </row>
+    <row r="71" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A71" s="5"/>
       <c r="B71" s="5"/>
       <c r="C71" s="5"/>
@@ -1349,8 +1415,9 @@
       <c r="F71" s="5"/>
       <c r="G71" s="5"/>
       <c r="H71" s="5"/>
-    </row>
-    <row r="72" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="I71" s="5"/>
+    </row>
+    <row r="72" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A72" s="5"/>
       <c r="B72" s="5"/>
       <c r="C72" s="5"/>
@@ -1359,6 +1426,7 @@
       <c r="F72" s="5"/>
       <c r="G72" s="5"/>
       <c r="H72" s="5"/>
+      <c r="I72" s="5"/>
     </row>
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>

</xml_diff>